<commit_message>
Customer tablolarının backend metotları yazıldı.
</commit_message>
<xml_diff>
--- a/GP1.xlsx
+++ b/GP1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="166">
   <si>
     <t>Stok</t>
   </si>
@@ -517,6 +517,12 @@
   </si>
   <si>
     <t>Cari Tanım(30)</t>
+  </si>
+  <si>
+    <t>Şirket(40)</t>
+  </si>
+  <si>
+    <t>Cari Grup(40)</t>
   </si>
 </sst>
 </file>
@@ -862,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,6 +1046,12 @@
       <c r="A31" t="s">
         <v>146</v>
       </c>
+      <c r="B31" t="s">
+        <v>165</v>
+      </c>
+      <c r="G31" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1056,9 +1068,6 @@
       <c r="C34" t="s">
         <v>137</v>
       </c>
-      <c r="G34" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1070,9 +1079,6 @@
       <c r="C35" t="s">
         <v>138</v>
       </c>
-      <c r="G35" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1084,9 +1090,6 @@
       <c r="C36" t="s">
         <v>139</v>
       </c>
-      <c r="G36" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1098,9 +1101,6 @@
       <c r="C37" t="s">
         <v>140</v>
       </c>
-      <c r="G37" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1112,7 +1112,29 @@
       <c r="C38" t="s">
         <v>141</v>
       </c>
-      <c r="G38" t="s">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1444,7 +1466,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Prefix,CustomerSubGroup,StockSubGroup tabloları eklendi ve düzenlemeler yapıldı.
</commit_message>
<xml_diff>
--- a/GP1.xlsx
+++ b/GP1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10380" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -870,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,7 +1149,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView zoomScale="127" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,7 +1466,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,7 +1694,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
CustomerSubGroup ve StockSubGroup backend metotları eklendi.
</commit_message>
<xml_diff>
--- a/GP1.xlsx
+++ b/GP1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10380" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="168">
   <si>
     <t>Stok</t>
   </si>
@@ -523,6 +523,12 @@
   </si>
   <si>
     <t>Cari Grup(40)</t>
+  </si>
+  <si>
+    <t>stok sub gruo(60)</t>
+  </si>
+  <si>
+    <t>Cari sub grup(50)</t>
   </si>
 </sst>
 </file>
@@ -868,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,84 +1063,92 @@
       <c r="A32" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>137</v>
-      </c>
-      <c r="B34" t="s">
-        <v>137</v>
-      </c>
-      <c r="C34" t="s">
-        <v>137</v>
+      <c r="B32" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>141</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>141</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G42" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1694,7 +1708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>

</xml_diff>